<commit_message>
开发ing add table [new] 设计表, 修改定义"_模板.xlsx"
</commit_message>
<xml_diff>
--- a/table/_模板.xlsx
+++ b/table/_模板.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dpace\HelloGo\grain_game\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D461387A-C656-4EE2-9BE7-6E3F0C25001F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83360369-0BEA-4396-8FB4-E1215A81338A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="title前六行" sheetId="1" r:id="rId1"/>
     <sheet name="解释" sheetId="2" r:id="rId2"/>
-    <sheet name="别名例子" sheetId="3" r:id="rId3"/>
-    <sheet name="数组子表例子" sheetId="4" r:id="rId4"/>
-    <sheet name="map子表例子" sheetId="5" r:id="rId5"/>
-    <sheet name="总表例子" sheetId="6" r:id="rId6"/>
-    <sheet name="总表例子-分表1" sheetId="7" r:id="rId7"/>
-    <sheet name="总表例子-分表2" sheetId="8" r:id="rId8"/>
+    <sheet name="=rare#别名例子" sheetId="3" r:id="rId3"/>
+    <sheet name="+subList#list子表" sheetId="4" r:id="rId4"/>
+    <sheet name="+subMap#map子表" sheetId="5" r:id="rId5"/>
+    <sheet name="总表A" sheetId="6" r:id="rId6"/>
+    <sheet name="总表A-分表1#分表例子" sheetId="7" r:id="rId7"/>
+    <sheet name="总表A-分表2#分表例子" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
   <si>
     <t>id</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -148,18 +148,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>分割符号为英文下的;</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>map的定义方式</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>k和v的分割符号为|,多个kv之间的分割为;【同数组的;】</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>带类型的定义方式</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -191,10 +183,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>关联(别名:表名.Sheet名)(子表:表名|sheet名)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>subList</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -231,22 +219,10 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>Shell名为aaa-bbb的表会被归为aaa的分表</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>总表-分表</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>注:表名可省略,表示本表,但"."不可省略</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>注:表名可省略,表示本表,但"|"不可省略</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>此类按程序自定义解析来配置，一般默认json格式</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -263,18 +239,58 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>title的第4行,格式为:表名.Sheet名字</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>title的第4行,格式为:表名|Sheet名字</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>index</t>
   </si>
   <si>
     <t>index</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>分割符号为英文下的|</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>k和v的分割符号为|,多个kv之间的分割为&amp;</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eg: 1|2|3|4</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eg: 1|a&amp;1|b&amp;2|c</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>title的第4行,格式为:表名+Sheet名字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>注:表名可省略,表示本表,但"+"不可省略</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>eg:同一个excel下的sheet, "道具-1","道具-2" 都合并到"道具"</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>同一个excel下的sheet, sheet名为aaa-bbb的表会被归为aaa的分表</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>*****</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>title的第4行,格式为:表名=Sheet名字</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>注:表名可省略,表示本表,但"="不可省略</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>关联(别名/子表/分表:参考页签:解释)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -657,13 +673,13 @@
   <dimension ref="B4:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="39.25" customWidth="1"/>
-    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.75" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.5" bestFit="1" customWidth="1"/>
@@ -726,10 +742,10 @@
         <v>10</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
@@ -770,10 +786,10 @@
         <v>21</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
@@ -802,14 +818,14 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -818,10 +834,10 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="O8" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -871,22 +887,25 @@
   <dimension ref="C10:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="60.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="10" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
@@ -894,48 +913,54 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>29</v>
+        <v>55</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>31</v>
+        <v>56</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
+        <v>31</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
@@ -943,24 +968,25 @@
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134DA431-901D-4FAA-A443-946204EA04C1}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -970,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -978,7 +1004,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -986,7 +1012,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -994,7 +1020,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1002,7 +1028,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1010,10 +1036,15 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1058,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1038,10 +1069,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1052,10 +1083,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1063,7 +1094,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1071,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1079,7 +1110,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1087,7 +1118,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1095,7 +1126,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1109,7 +1140,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1119,13 +1150,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1142,7 +1173,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1211,7 +1242,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1322,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1371,7 +1402,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="L39" sqref="L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
开发ing add table [new] 设计表, 修改定义"_模板.xlsx" 1
</commit_message>
<xml_diff>
--- a/table/_模板.xlsx
+++ b/table/_模板.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dpace\HelloGo\grain_game\table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83360369-0BEA-4396-8FB4-E1215A81338A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C6A526-11A9-4222-9C90-F68FA37D1D91}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="title前六行" sheetId="1" r:id="rId1"/>
     <sheet name="解释" sheetId="2" r:id="rId2"/>
-    <sheet name="=rare#别名例子" sheetId="3" r:id="rId3"/>
-    <sheet name="+subList#list子表" sheetId="4" r:id="rId4"/>
-    <sheet name="+subMap#map子表" sheetId="5" r:id="rId5"/>
+    <sheet name="$表名=rare#别名例子" sheetId="3" r:id="rId3"/>
+    <sheet name="$表名+subList#list子表" sheetId="4" r:id="rId4"/>
+    <sheet name="$表名+subMap#map子表" sheetId="5" r:id="rId5"/>
     <sheet name="总表A" sheetId="6" r:id="rId6"/>
     <sheet name="总表A-分表1#分表例子" sheetId="7" r:id="rId7"/>
     <sheet name="总表A-分表2#分表例子" sheetId="8" r:id="rId8"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="70">
   <si>
     <t>id</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -227,10 +227,6 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>表名(可省略).别名例子</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>表名(可省略)|数组子表例子</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
@@ -291,6 +287,22 @@
   </si>
   <si>
     <t>关联(别名/子表/分表:参考页签:解释)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>a|b|c</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>a|1&amp;b|2&amp;c|3</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>表名(可省略)=别名例子</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -673,7 +685,7 @@
   <dimension ref="B4:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -800,7 +812,9 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="H7" s="1">
         <v>99999999</v>
       </c>
@@ -813,19 +827,23 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="N7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -834,10 +852,10 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
@@ -879,6 +897,7 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -902,10 +921,10 @@
         <v>48</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
@@ -913,10 +932,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.2">
@@ -924,10 +943,10 @@
         <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.2">
@@ -946,10 +965,10 @@
         <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
@@ -957,10 +976,10 @@
         <v>38</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
@@ -968,10 +987,10 @@
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1063,7 @@
     </row>
     <row r="30" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1069,7 +1088,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
@@ -1140,7 +1159,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1150,7 +1169,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>46</v>

</xml_diff>